<commit_message>
Desenvolvimento de fluxos para cliente nacional e internacional
</commit_message>
<xml_diff>
--- a/Plano_Preparação_NET_2021.xlsx
+++ b/Plano_Preparação_NET_2021.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fabiano\Desktop\ARQUIVOS\Estudo estágio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FOEU\My Private Documents\Plano de Estudos UBS BB\projetos\projetoProspeccao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B58E7380-D2CA-4EB7-9963-D57F6994B36A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B67194DA-3B7D-4395-B2CD-7A6C1DDB790C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Calibragem conhecimento" sheetId="7" r:id="rId1"/>
@@ -315,10 +315,10 @@
     <t>OK</t>
   </si>
   <si>
-    <t>Estórias 5 e 6 - Console com login e fluxo básico (cadastro de cliente nacional, aprovação da gerência) e fluxo internacional</t>
-  </si>
-  <si>
     <t>Feito</t>
+  </si>
+  <si>
+    <t>Estórias 5 e 6 - Console com login e fluxo básico (cadastro de cliente nacional, aprovação da gerência) e fluxo internacional, reprovação e correção de cadastro</t>
   </si>
 </sst>
 </file>
@@ -746,7 +746,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B53AE3B-2636-4E78-BB56-74436ABD7491}">
   <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -1048,8 +1048,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1098,7 +1098,7 @@
         <v>44532</v>
       </c>
       <c r="F2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1118,7 +1118,7 @@
         <v>52</v>
       </c>
       <c r="F3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1138,7 +1138,7 @@
         <v>53</v>
       </c>
       <c r="F4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1158,7 +1158,7 @@
         <v>44319</v>
       </c>
       <c r="F5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1169,7 +1169,7 @@
         <v>8</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D6" s="1">
         <v>44411</v>

</xml_diff>